<commit_message>
Initial treatise for attributes
</commit_message>
<xml_diff>
--- a/install sql/Generate UPDATE sql with real values.xlsx
+++ b/install sql/Generate UPDATE sql with real values.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Structured-Data-for-Zen-Cart\install sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\zen-cart_Structured-Data\install sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CDCEE8-907D-47CB-8F4E-F34413320513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="0" windowWidth="19350" windowHeight="8340"/>
+    <workbookView xWindow="-27990" yWindow="-9495" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Your values" sheetId="1" r:id="rId1"/>
     <sheet name="SQL to copy and paste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -168,9 +178,6 @@
     <t>PLUGIN_SDATA_ELIGIBLE_REGION</t>
   </si>
   <si>
-    <t>PLUGIN_SDATA_PRICE_CURRRENCY</t>
-  </si>
-  <si>
     <t>PLUGIN_SDATA_DELIVERYLEADTIME</t>
   </si>
   <si>
@@ -222,15 +229,6 @@
     <t>Enable Structured Data processing code and display of markup groups? This is a global option.</t>
   </si>
   <si>
-    <t>Show Schema markup?&lt;br /&gt;Shows JSON-LD blocks for Organisation and Breadcrumbs on all pages</t>
-  </si>
-  <si>
-    <t>Show Facebook-Open Graph markup?&lt;br /&gt;Shows Facebook og tags on all pages with additional product-specific tags on product pages.</t>
-  </si>
-  <si>
-    <t>Show Twitter Card markup?&lt;br /&gt;Shows on all pages.</t>
-  </si>
-  <si>
     <t>Enter your Facebook application ID (&lt;a href="http://developers.facebook.com/setup/" target="_blank"&gt;Get an application ID&lt;/a&gt;).</t>
   </si>
   <si>
@@ -297,9 +295,6 @@
     <t>The Dun &amp; Bradstreet DUNS number for identifying an organization or business person.</t>
   </si>
   <si>
-    <t>The geographical region served (&lt;a href="https://schema.org/areaServed" target="_blank"&gt;further details here&lt;/a&gt;).&lt;br /&gt;If omitted assumed worldwide.</t>
-  </si>
-  <si>
     <t>Fallback image used when there is no product image. Enter the full url or leave blank to use the no-image file defined in the Admin-&gt;Images configuration.</t>
   </si>
   <si>
@@ -336,19 +331,34 @@
     <t>PLUGIN_SDATA_DELIVERYLEADTIME_OOS</t>
   </si>
   <si>
-    <t>Enter a list of urls to other (NOT Facebook, Twitter or Google Plus) profile or social pages related to your business (eg. Linked In, Dun &amp; Bradstreet, Yelp etc.).&lt;br /&gt;Separate the urls with commas.</t>
-  </si>
-  <si>
     <t>Value - ENTER YOUR VALUES HERE</t>
   </si>
   <si>
     <t>1,en_GB</t>
+  </si>
+  <si>
+    <t>PLUGIN_SDATA_PRICE_CURRENCY</t>
+  </si>
+  <si>
+    <t>Show Schema markup?&lt;br&gt;Shows JSON-LD blocks for Organisation and Breadcrumbs on all pages</t>
+  </si>
+  <si>
+    <t>Show Facebook-Open Graph markup?&lt;br&gt;Shows Facebook og tags on all pages with additional product-specific tags on product pages.</t>
+  </si>
+  <si>
+    <t>Show Twitter Card markup?&lt;br&gt;Shows on all pages.</t>
+  </si>
+  <si>
+    <t>Enter a list of urls to other (NOT Facebook, Twitter or Google Plus) profile or social pages related to your business (eg. Linked In, Dun &amp; Bradstreet, Yelp etc.).&lt;br&gt;Separate the urls with commas.</t>
+  </si>
+  <si>
+    <t>The geographical region served (&lt;a href="https://schema.org/areaServed" target="_blank"&gt;further details here&lt;/a&gt;).&lt;br&gt;If omitted assumed worldwide.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -672,26 +682,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="61" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="61" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="61" style="1"/>
+    <col min="1" max="1" width="27.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="5.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="61" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
@@ -700,247 +729,247 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="36" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="24" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="84" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1003,343 +1032,343 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="24" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="48" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="36" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="36" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="48" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="36" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="36" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A1:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="149.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="186.21875" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A2&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C2&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_ENABLE';</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A3&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C3&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_SCHEMA_ENABLE';</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A4&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C4&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ENABLE';</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A5&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C5&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_CARD_ENABLE';</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A6&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C6&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_APPID';</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A7&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C7&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ADMINID';</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A8&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C8&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PAGE';</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A9&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C9&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LOGO';</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A10&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C10&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_STREET_ADDRESS';</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A11&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C11&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LOCALITY';</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A12&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C12&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_REGION';</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A13&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C13&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_POSTALCODE';</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A14&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C14&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_COUNTRYNAME';</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A15&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C15&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_EMAIL';</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A16&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C16&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TELEPHONE';</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A17&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C17&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FAX';</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A18&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C18&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_AVAILABLE_LANGUAGE';</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A19&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C19&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '1,en_GB' WHERE configuration_key = 'PLUGIN_SDATA_FOG_LOCALES';</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A20&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C20&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TAXID';</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A21&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C21&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_VATID';</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A22&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C22&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_SAMEAS';</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A23&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C23&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_ELIGIBLE_REGION';</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A24&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C24&amp;"'"&amp;";")</f>
-        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_PRICE_CURRRENCY';</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_PRICE_CURRENCY';</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A25&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C25&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '2' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME';</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A26&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C26&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '7' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME_OOS';</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A27&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C27&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'new' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PRODUCT_CONDITION';</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A28&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C28&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' ByBankTransferInAdvance,  COD, PayPal, AmericanExpress, MasterCard, VISA' WHERE configuration_key = 'PLUGIN_SDATA_ACCEPTED_PAYMENT_METHODS';</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A29&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C29&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LEGAL_NAME';</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A30&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C30&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_DUNS';</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A31&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C31&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_AREA_SERVED';</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A32&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C32&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_PRODUCT_IMAGE';</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A33&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C33&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_IMAGE';</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A34&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C34&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' business.business' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_SITE';</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A35&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C35&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' product' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_PRODUCT';</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A36&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C36&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_DEFAULT_IMAGE';</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A37&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C37&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_USERNAME';</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A38&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C38&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_PAGE';</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A39&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C39&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_GOOGLE_PUBLISHER';</v>

</xml_diff>

<commit_message>
update for google product category
</commit_message>
<xml_diff>
--- a/install sql/Generate UPDATE sql with real values.xlsx
+++ b/install sql/Generate UPDATE sql with real values.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\zen-cart_Structured-Data\install sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CDCEE8-907D-47CB-8F4E-F34413320513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62875416-E8BD-4900-AC9C-9660E59DAD6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-9495" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-105" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Your values" sheetId="1" r:id="rId1"/>
-    <sheet name="SQL to copy and paste" sheetId="2" r:id="rId2"/>
+    <sheet name="Production values" sheetId="1" r:id="rId1"/>
+    <sheet name="Production SQL" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Values" sheetId="3" r:id="rId3"/>
+    <sheet name="Test SQL" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,64 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
-  <si>
-    <t xml:space="preserve"> @configuration_group_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NOW()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NULL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ByInvoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cash</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CheckInAdvance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DirectDebit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GoogleCheckout</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PayPal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PaySwarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AmericanExpress</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DinersClub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Discover</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MasterCard</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VISA'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VISA.'</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
   <si>
     <t>true</t>
   </si>
@@ -353,6 +298,63 @@
   </si>
   <si>
     <t>The geographical region served (&lt;a href="https://schema.org/areaServed" target="_blank"&gt;further details here&lt;/a&gt;).&lt;br&gt;If omitted assumed worldwide.</t>
+  </si>
+  <si>
+    <t>123456879</t>
+  </si>
+  <si>
+    <t>admin_myfacebook_page</t>
+  </si>
+  <si>
+    <t>www.myfacebook.com</t>
+  </si>
+  <si>
+    <t>www.mywebsite.com/logo.jpg</t>
+  </si>
+  <si>
+    <t>MyTown</t>
+  </si>
+  <si>
+    <t>MyState</t>
+  </si>
+  <si>
+    <t>MyStreetAddress 1</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>MyCountry</t>
+  </si>
+  <si>
+    <t>myemailaddress@mywebsite.com</t>
+  </si>
+  <si>
+    <t>+44 123456789</t>
+  </si>
+  <si>
+    <t>+44 123456780</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>GB123546789</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>MyCompanyName</t>
+  </si>
+  <si>
+    <t>myTwitterName</t>
+  </si>
+  <si>
+    <t>https://myTwitterpage</t>
   </si>
 </sst>
 </file>
@@ -395,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -403,6 +405,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,11 +686,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -720,410 +723,350 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="24" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="24" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" ht="36" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="24" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U28" s="1">
-        <v>28</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +1080,7 @@
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A1:A38"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,229 +1091,229 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A2&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C2&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A2&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C2&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_ENABLE';</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A3&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C3&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A3&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C3&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_SCHEMA_ENABLE';</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A4&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C4&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A4&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C4&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ENABLE';</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A5&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C5&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A5&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C5&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_CARD_ENABLE';</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A6&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C6&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A6&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C6&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_APPID';</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A7&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C7&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A7&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C7&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ADMINID';</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A8&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C8&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A8&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C8&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PAGE';</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A9&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C9&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A9&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C9&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LOGO';</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A10&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C10&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A10&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C10&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_STREET_ADDRESS';</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A11&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C11&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A11&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C11&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LOCALITY';</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A12&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C12&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A12&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C12&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_REGION';</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A13&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C13&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A13&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C13&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_POSTALCODE';</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A14&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C14&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A14&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C14&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_COUNTRYNAME';</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A15&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C15&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A15&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C15&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_EMAIL';</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A16&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C16&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A16&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C16&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TELEPHONE';</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A17&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C17&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A17&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C17&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FAX';</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A18&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C18&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A18&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C18&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_AVAILABLE_LANGUAGE';</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A19&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C19&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A19&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C19&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '1,en_GB' WHERE configuration_key = 'PLUGIN_SDATA_FOG_LOCALES';</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A20&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C20&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A20&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C20&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TAXID';</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A21&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C21&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A21&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C21&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_VATID';</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A22&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C22&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A22&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C22&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_SAMEAS';</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A23&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C23&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A23&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C23&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_ELIGIBLE_REGION';</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A24&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C24&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A24&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C24&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_PRICE_CURRENCY';</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A25&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C25&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A25&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C25&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '2' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME';</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A26&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C26&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A26&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C26&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '7' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME_OOS';</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A27&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C27&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A27&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C27&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = 'new' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PRODUCT_CONDITION';</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A28&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C28&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A28&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C28&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' ByBankTransferInAdvance,  COD, PayPal, AmericanExpress, MasterCard, VISA' WHERE configuration_key = 'PLUGIN_SDATA_ACCEPTED_PAYMENT_METHODS';</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A29&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C29&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A29&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C29&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_LEGAL_NAME';</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A30&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C30&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A30&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C30&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_DUNS';</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A31&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C31&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A31&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C31&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_AREA_SERVED';</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A32&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C32&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A32&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C32&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_PRODUCT_IMAGE';</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A33&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C33&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A33&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C33&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_IMAGE';</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A34&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C34&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A34&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C34&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' business.business' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_SITE';</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A35&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C35&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A35&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C35&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = ' product' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_PRODUCT';</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A36&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C36&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A36&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C36&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_DEFAULT_IMAGE';</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A37&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C37&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A37&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C37&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_USERNAME';</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A38&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C38&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A38&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C38&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_PAGE';</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Your values'!A39&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Your values'!C39&amp;"'"&amp;";")</f>
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Production values'!A39&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Production values'!C39&amp;"'"&amp;";")</f>
         <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_GOOGLE_PUBLISHER';</v>
       </c>
     </row>
@@ -1378,4 +1321,676 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AC4971-417E-4514-AC3F-55D312E4C53A}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3112D32D-72C5-47F2-9E64-89585BA3DD2F}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="182" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A2&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C2&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_ENABLE';</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A3&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C3&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_SCHEMA_ENABLE';</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A4&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C4&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ENABLE';</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A5&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C5&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'true' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_CARD_ENABLE';</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A6&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C6&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '123456879' WHERE configuration_key = 'PLUGIN_SDATA_FOG_APPID';</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A7&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C7&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'admin_myfacebook_page' WHERE configuration_key = 'PLUGIN_SDATA_FOG_ADMINID';</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A8&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C8&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'www.myfacebook.com' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PAGE';</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A9&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C9&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'www.mywebsite.com/logo.jpg' WHERE configuration_key = 'PLUGIN_SDATA_LOGO';</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A10&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C10&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'MyStreetAddress 1' WHERE configuration_key = 'PLUGIN_SDATA_STREET_ADDRESS';</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A11&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C11&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'MyTown' WHERE configuration_key = 'PLUGIN_SDATA_LOCALITY';</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A12&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C12&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'MyState' WHERE configuration_key = 'PLUGIN_SDATA_REGION';</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A13&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C13&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '123456' WHERE configuration_key = 'PLUGIN_SDATA_POSTALCODE';</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A14&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C14&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'MyCountry' WHERE configuration_key = 'PLUGIN_SDATA_COUNTRYNAME';</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A15&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C15&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'myemailaddress@mywebsite.com' WHERE configuration_key = 'PLUGIN_SDATA_EMAIL';</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A16&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C16&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '+44 123456789' WHERE configuration_key = 'PLUGIN_SDATA_TELEPHONE';</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A17&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C17&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '+44 123456780' WHERE configuration_key = 'PLUGIN_SDATA_FAX';</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A18&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C18&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'english' WHERE configuration_key = 'PLUGIN_SDATA_AVAILABLE_LANGUAGE';</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A19&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C19&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '1,en_GB' WHERE configuration_key = 'PLUGIN_SDATA_FOG_LOCALES';</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A20&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C20&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '123456789' WHERE configuration_key = 'PLUGIN_SDATA_TAXID';</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A21&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C21&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'GB123546789' WHERE configuration_key = 'PLUGIN_SDATA_VATID';</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A22&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C22&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_SAMEAS';</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A23&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C23&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_ELIGIBLE_REGION';</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A24&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C24&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'GBP' WHERE configuration_key = 'PLUGIN_SDATA_PRICE_CURRENCY';</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A25&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C25&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '2' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME';</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A26&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C26&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '7' WHERE configuration_key = 'PLUGIN_SDATA_DELIVERYLEADTIME_OOS';</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A27&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C27&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'new' WHERE configuration_key = 'PLUGIN_SDATA_FOG_PRODUCT_CONDITION';</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A28&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C28&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = ' ByBankTransferInAdvance,  COD, PayPal, AmericanExpress, MasterCard, VISA' WHERE configuration_key = 'PLUGIN_SDATA_ACCEPTED_PAYMENT_METHODS';</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A29&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C29&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'MyCompanyName' WHERE configuration_key = 'PLUGIN_SDATA_LEGAL_NAME';</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A30&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C30&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_DUNS';</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A31&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C31&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_AREA_SERVED';</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A32&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C32&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_PRODUCT_IMAGE';</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A33&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C33&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_FOG_DEFAULT_IMAGE';</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A34&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C34&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = ' business.business' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_SITE';</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A35&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C35&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = ' product' WHERE configuration_key = 'PLUGIN_SDATA_FOG_TYPE_PRODUCT';</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A36&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C36&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_DEFAULT_IMAGE';</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A37&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C37&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'myTwitterName' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_USERNAME';</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A38&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C38&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = 'https://myTwitterpage' WHERE configuration_key = 'PLUGIN_SDATA_TWITTER_PAGE';</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>CLEAN("UPDATE configuration SET configuration_value = '"&amp;'Test Values'!A39&amp;"'"&amp;" WHERE configuration_key = '"&amp;'Test Values'!C39&amp;"'"&amp;";")</f>
+        <v>UPDATE configuration SET configuration_value = '' WHERE configuration_key = 'PLUGIN_SDATA_GOOGLE_PUBLISHER';</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>